<commit_message>
📝 nuevos datos intersedes
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/1EncuentroIntersedesVrt_CategorizacionVisualizacionCSLMR_20240906.xlsx
+++ b/aplicaciones/procesador/datos/1EncuentroIntersedesVrt_CategorizacionVisualizacionCSLMR_20240906.xlsx
@@ -445,7 +445,7 @@
     <t>[…] Pero ¿qué está ocurriendo? están siendo masacradas, desplazadas, se están contaminando de esta cultura occidental que en realidad no les aporta mucho, yo he hecho trabajo de campo en la zona y, es lamentable ver niños usando bóxer y pidiendo dinero, entonces a lo que voy es que, con lo que plantea el profesor WADA sí, no debemos apuntar solo a que deba ser conocimiento de punta patente eso, eso lo tengo claro. […]</t>
   </si>
   <si>
-    <t>CONTEXTO CULTURAL</t>
+    <t>CONTEXTO SOCIOCULTURAL</t>
   </si>
   <si>
     <t>[…] Pero tampoco la Universidad debe renunciar a eso, debemos movernos entre esos mundos y también un mundo del conocimiento cotidiano que puede ser muy profundo, sí. El diálogo con la selva, con los bosques, repito, lo que hacen comunidades aborígenes ancestrales, técnicas constructivas, incluso entonces manejo del agua, manejo de semillas, es una cuestión supremamente importante y yo creo que nuestra Universidad ha hecho esfuerzos al respecto, pero deberían ser más sólidos. No solo el conocimiento más necesario está en la High Tech, puede estar al frente y no lo vemos y Colombia tiene mucho de ancestralidad, mucho de adaptación a los Andes, cambio climático y tal. […]</t>
@@ -2833,7 +2833,7 @@
       <c r="F51" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G51" s="16" t="s">
         <v>106</v>
       </c>
       <c r="H51" s="23" t="s">

</xml_diff>